<commit_message>
Merged a bunch in to MSS_PARTs, though still a mess Updated Resistors, caps, electromec and magnetics
</commit_message>
<xml_diff>
--- a/Data/Electromechanical.xlsx
+++ b/Data/Electromechanical.xlsx
@@ -9,23 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19950" windowHeight="7710" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19950" windowHeight="7710" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Jacks" sheetId="1" r:id="rId1"/>
-    <sheet name="Plugs" sheetId="4" r:id="rId2"/>
+    <sheet name="EXT-Jacks" sheetId="1" r:id="rId1"/>
+    <sheet name="EXT-Plugs" sheetId="4" r:id="rId2"/>
     <sheet name="Switches" sheetId="2" r:id="rId3"/>
-    <sheet name="Connectors" sheetId="3" r:id="rId4"/>
+    <sheet name="INT-Connectors" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="36">
-  <si>
-    <t>Part Number</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="38">
   <si>
     <t>Type</t>
   </si>
@@ -130,6 +127,15 @@
   </si>
   <si>
     <t>SPST High Power Switch, 125VAC, 11A, Quick Connect, Panel Mount</t>
+  </si>
+  <si>
+    <t>..\Schematic\Symbols.SchLib</t>
+  </si>
+  <si>
+    <t>..\PCB\footprints.PcbLib</t>
+  </si>
+  <si>
+    <t>Local Part Number</t>
   </si>
 </sst>
 </file>
@@ -169,9 +175,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,13 +490,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="49" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="26.7109375" bestFit="1" customWidth="1"/>
@@ -497,96 +505,108 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
       <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
         <v>15</v>
       </c>
-      <c r="L1" t="s">
-        <v>16</v>
-      </c>
       <c r="M1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
-        <v>13</v>
+      <c r="E2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="H2" t="b">
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" t="s">
         <v>17</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>18</v>
-      </c>
-      <c r="L2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="H3" t="b">
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" t="s">
         <v>21</v>
-      </c>
-      <c r="K3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -600,7 +620,7 @@
   <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -620,44 +640,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
       <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
         <v>15</v>
       </c>
-      <c r="L1" t="s">
-        <v>16</v>
-      </c>
       <c r="M1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -669,107 +689,119 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="61.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
       <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
         <v>15</v>
       </c>
-      <c r="L1" t="s">
-        <v>16</v>
-      </c>
       <c r="M1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="H2" t="b">
         <v>0</v>
       </c>
       <c r="I2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" t="s">
         <v>28</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" t="s">
         <v>30</v>
-      </c>
-      <c r="L2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
         <v>24</v>
       </c>
-      <c r="B3" t="s">
-        <v>25</v>
-      </c>
       <c r="C3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>35</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="H3" t="b">
         <v>0</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -782,48 +814,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
       <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
         <v>15</v>
-      </c>
-      <c r="L1" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add a bunch of databases
</commit_message>
<xml_diff>
--- a/Data/Electromechanical.xlsx
+++ b/Data/Electromechanical.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="132">
   <si>
     <t>Type</t>
   </si>
@@ -163,6 +163,261 @@
   </si>
   <si>
     <t>Power-IEC</t>
+  </si>
+  <si>
+    <t>3PDT Footswitch</t>
+  </si>
+  <si>
+    <t>Alpha</t>
+  </si>
+  <si>
+    <t>SF17020F-0302-21R-L</t>
+  </si>
+  <si>
+    <t>3PDT Footswitch Latching Solder Tabs</t>
+  </si>
+  <si>
+    <t>SW-3PDT</t>
+  </si>
+  <si>
+    <t>DPDT Footswitch</t>
+  </si>
+  <si>
+    <t>SF12020F-0202-20R-L-011</t>
+  </si>
+  <si>
+    <t>DPDT Footswitch Latching with Solder Pins</t>
+  </si>
+  <si>
+    <t>SW-DPDT</t>
+  </si>
+  <si>
+    <t>Jack 2.1mm barrel</t>
+  </si>
+  <si>
+    <t>Kobiconn</t>
+  </si>
+  <si>
+    <t>163-4302-E</t>
+  </si>
+  <si>
+    <t>Panel Mount 2.1mm ID, 5.5mm OD</t>
+  </si>
+  <si>
+    <t>163-7620E-E</t>
+  </si>
+  <si>
+    <t>PCB Mount 2.1mm ID, 5.5mm OD</t>
+  </si>
+  <si>
+    <t>Right Angle PCB Mount TRS with removable nose</t>
+  </si>
+  <si>
+    <t>NMJ6HCD2</t>
+  </si>
+  <si>
+    <t>Neutrik</t>
+  </si>
+  <si>
+    <t>Jack TRS-RN</t>
+  </si>
+  <si>
+    <t>Right Angle PCB Mount TS with removable nose</t>
+  </si>
+  <si>
+    <t>NMJ4HCD2</t>
+  </si>
+  <si>
+    <t>Jack TS-RN</t>
+  </si>
+  <si>
+    <t>Right Angle PCB Mount TRS Normaled</t>
+  </si>
+  <si>
+    <t>NRJ6HF</t>
+  </si>
+  <si>
+    <t>Jack TRS-N</t>
+  </si>
+  <si>
+    <t>Right Angle PCB Mount TS Normaled</t>
+  </si>
+  <si>
+    <t>NRJ4HF</t>
+  </si>
+  <si>
+    <t>Jack TS-N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vertical PCB Mount TRS </t>
+  </si>
+  <si>
+    <t>NYS2343</t>
+  </si>
+  <si>
+    <t>Jack TRS-RA</t>
+  </si>
+  <si>
+    <t>Vertical PCB Mount TRS Normaled</t>
+  </si>
+  <si>
+    <t>NYS234</t>
+  </si>
+  <si>
+    <t>Jack TRS-S-RA</t>
+  </si>
+  <si>
+    <t>Open Frame Panel Mount TRS Shorting</t>
+  </si>
+  <si>
+    <t>14B</t>
+  </si>
+  <si>
+    <t>Jack TRS-S</t>
+  </si>
+  <si>
+    <t>Open Frame Panel Mount TS Shorting</t>
+  </si>
+  <si>
+    <t>12A</t>
+  </si>
+  <si>
+    <t>Jack TS-S</t>
+  </si>
+  <si>
+    <t>Open Frame Panel Mount TRS</t>
+  </si>
+  <si>
+    <t>12B</t>
+  </si>
+  <si>
+    <t>Jack TRS</t>
+  </si>
+  <si>
+    <t>Open Frame Panel Mount TS</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>Jack TS</t>
+  </si>
+  <si>
+    <t>Jack XLR-MP</t>
+  </si>
+  <si>
+    <t>NC3MD-L-B-1</t>
+  </si>
+  <si>
+    <t>Panel Mount XLR Male</t>
+  </si>
+  <si>
+    <t>Jack XLR-FP</t>
+  </si>
+  <si>
+    <t>NC3FD-L-B-1</t>
+  </si>
+  <si>
+    <t>Panel Mount XLR Female</t>
+  </si>
+  <si>
+    <t>Jack XLR-Combo</t>
+  </si>
+  <si>
+    <t>NCJ6FA-H</t>
+  </si>
+  <si>
+    <t>Panel Mount XLR - TRS Combo</t>
+  </si>
+  <si>
+    <t>Jack XLR-MB</t>
+  </si>
+  <si>
+    <t>NC3MAH</t>
+  </si>
+  <si>
+    <t>PCB Mount XLR Male</t>
+  </si>
+  <si>
+    <t>Jack XLR-FB</t>
+  </si>
+  <si>
+    <t>NC3FAH</t>
+  </si>
+  <si>
+    <t>PCB Mount XLR Female</t>
+  </si>
+  <si>
+    <t>Jack 1/8" TRS-P</t>
+  </si>
+  <si>
+    <t>Amphenol</t>
+  </si>
+  <si>
+    <t>ACJS-MV35-3S</t>
+  </si>
+  <si>
+    <t>Panel Mount 1/8" TRS</t>
+  </si>
+  <si>
+    <t>Jack 1/8" TRS-B</t>
+  </si>
+  <si>
+    <t>35RASMT4BHNTRX</t>
+  </si>
+  <si>
+    <t>PCB Mount 1/8" TRS Normaled</t>
+  </si>
+  <si>
+    <t>Jack 1/8" TRS-BN</t>
+  </si>
+  <si>
+    <t>35RASMT2BHNTRX</t>
+  </si>
+  <si>
+    <t>PCB Mount 1/8" TRS</t>
+  </si>
+  <si>
+    <t>Jack RCA-Dual-H</t>
+  </si>
+  <si>
+    <t>PJRAS2X1S01X</t>
+  </si>
+  <si>
+    <t>Dual RCA - Horizontal</t>
+  </si>
+  <si>
+    <t>Jack RCA-Dual-V</t>
+  </si>
+  <si>
+    <t>PJRAS1X2S01AUX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dual RCA - Vertical </t>
+  </si>
+  <si>
+    <t>PNL-19mmx12.9mmx11.6mm</t>
+  </si>
+  <si>
+    <t>0.25 Quick-Disconnect Tabs, SPST</t>
+  </si>
+  <si>
+    <t>Power Switch, SPST, 0.25 Q.D. tabs, Panel Mount</t>
+  </si>
+  <si>
+    <t>Switch SPST</t>
+  </si>
+  <si>
+    <t>..\Schematic\basic_components.SchLib</t>
+  </si>
+  <si>
+    <t>PJRAS1X2S01X </t>
+  </si>
+  <si>
+    <t>Red/White inserts, Nickle Plated</t>
+  </si>
+  <si>
+    <t>RCA Jack Dual Vertical Stack Red / White Inserts</t>
   </si>
 </sst>
 </file>
@@ -202,11 +457,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,15 +772,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="49" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
@@ -674,6 +932,325 @@
       </c>
       <c r="L3" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C26" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -754,9 +1331,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -766,7 +1345,7 @@
     <col min="12" max="12" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
@@ -807,7 +1386,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -839,7 +1418,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -870,6 +1449,71 @@
       <c r="L3" t="s">
         <v>30</v>
       </c>
+    </row>
+    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="N6" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updates for electro-mech and ICs
</commit_message>
<xml_diff>
--- a/Data/Electromechanical.xlsx
+++ b/Data/Electromechanical.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt.sterling\Documents\MSS\library\trunk\Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19950" windowHeight="7710" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19950" windowHeight="7710"/>
   </bookViews>
   <sheets>
     <sheet name="EXT-Jacks" sheetId="1" r:id="rId1"/>
@@ -483,9 +478,6 @@
     <t>1/4" TRS Jack Normaled Vertical PCB Mount</t>
   </si>
   <si>
-    <t xml:space="preserve">1/4" TRS Jack Normaled Vertical PCB Mount </t>
-  </si>
-  <si>
     <t>1/4" TRS Jack Normaled Right Angle PCB Mount</t>
   </si>
   <si>
@@ -547,13 +539,16 @@
   </si>
   <si>
     <t>JST-PH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/4" TRS Jack Un-Normaled Vertical PCB Mount </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -640,14 +635,6 @@
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
   </tableStyles>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -906,21 +893,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="3" max="3" width="21.28515625" customWidth="1"/>
     <col min="4" max="4" width="56.42578125" bestFit="1" customWidth="1"/>
@@ -940,7 +927,7 @@
     <col min="19" max="19" width="24.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" ht="12.75">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
@@ -999,7 +986,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="15.75" customHeight="1">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1055,7 +1042,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" ht="15.75" customHeight="1">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1096,7 +1083,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" ht="15.75" customHeight="1">
       <c r="A4" t="s">
         <v>108</v>
       </c>
@@ -1128,7 +1115,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" ht="15.75" customHeight="1">
       <c r="A5" t="s">
         <v>109</v>
       </c>
@@ -1160,7 +1147,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" ht="15.75" customHeight="1">
       <c r="A6" t="s">
         <v>110</v>
       </c>
@@ -1192,7 +1179,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" ht="15.75" customHeight="1">
       <c r="A7" t="s">
         <v>111</v>
       </c>
@@ -1224,7 +1211,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" ht="15.75" customHeight="1">
       <c r="A8" t="s">
         <v>112</v>
       </c>
@@ -1256,7 +1243,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" ht="15.75" customHeight="1">
       <c r="A9" t="s">
         <v>113</v>
       </c>
@@ -1288,7 +1275,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" ht="15.75" customHeight="1">
       <c r="A10" t="s">
         <v>114</v>
       </c>
@@ -1320,7 +1307,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" ht="15.75" customHeight="1">
       <c r="A11" t="s">
         <v>115</v>
       </c>
@@ -1334,7 +1321,7 @@
         <v>142</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>153</v>
+        <v>174</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>33</v>
@@ -1352,7 +1339,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" ht="15.75" customHeight="1">
       <c r="A12" t="s">
         <v>116</v>
       </c>
@@ -1384,7 +1371,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" ht="15.75" customHeight="1">
       <c r="A13" t="s">
         <v>117</v>
       </c>
@@ -1398,7 +1385,7 @@
         <v>145</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>33</v>
@@ -1416,7 +1403,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" ht="15.75" customHeight="1">
       <c r="A14" t="s">
         <v>118</v>
       </c>
@@ -1430,7 +1417,7 @@
         <v>148</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>33</v>
@@ -1448,7 +1435,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" ht="15.75" customHeight="1">
       <c r="A15" t="s">
         <v>119</v>
       </c>
@@ -1462,7 +1449,7 @@
         <v>148</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>33</v>
@@ -1480,7 +1467,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" ht="15.75" customHeight="1">
       <c r="A16" t="s">
         <v>120</v>
       </c>
@@ -1492,7 +1479,7 @@
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>33</v>
@@ -1510,7 +1497,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" ht="15.75" customHeight="1">
       <c r="A17" t="s">
         <v>121</v>
       </c>
@@ -1522,7 +1509,7 @@
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>33</v>
@@ -1540,7 +1527,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" ht="15.75" customHeight="1">
       <c r="A18" t="s">
         <v>122</v>
       </c>
@@ -1552,7 +1539,7 @@
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>33</v>
@@ -1570,7 +1557,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" ht="15.75" customHeight="1">
       <c r="A19" t="s">
         <v>123</v>
       </c>
@@ -1582,7 +1569,7 @@
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>33</v>
@@ -1600,7 +1587,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" ht="15.75" customHeight="1">
       <c r="A20" t="s">
         <v>124</v>
       </c>
@@ -1612,7 +1599,7 @@
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>33</v>
@@ -1630,7 +1617,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" ht="15.75" customHeight="1">
       <c r="A21" t="s">
         <v>125</v>
       </c>
@@ -1642,7 +1629,7 @@
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>33</v>
@@ -1660,7 +1647,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" ht="15.75" customHeight="1">
       <c r="A22" t="s">
         <v>126</v>
       </c>
@@ -1672,7 +1659,7 @@
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>33</v>
@@ -1690,7 +1677,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" ht="15.75" customHeight="1">
       <c r="A23" t="s">
         <v>127</v>
       </c>
@@ -1702,7 +1689,7 @@
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>33</v>
@@ -1720,7 +1707,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" ht="15.75" customHeight="1">
       <c r="A24" t="s">
         <v>128</v>
       </c>
@@ -1732,7 +1719,7 @@
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>33</v>
@@ -1750,7 +1737,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" ht="15.75" customHeight="1">
       <c r="A25" t="s">
         <v>129</v>
       </c>
@@ -1762,7 +1749,7 @@
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>33</v>
@@ -1780,7 +1767,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" ht="15.75" customHeight="1">
       <c r="A26" t="s">
         <v>130</v>
       </c>
@@ -1794,7 +1781,7 @@
         <v>101</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>33</v>
@@ -1820,14 +1807,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
@@ -1843,7 +1830,7 @@
     <col min="12" max="12" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
@@ -1884,18 +1871,18 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>107</v>
       </c>
       <c r="C2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>33</v>
@@ -1908,14 +1895,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="61.140625" bestFit="1" customWidth="1"/>
@@ -1925,7 +1912,7 @@
     <col min="12" max="12" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
@@ -1966,7 +1953,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="15.75" customHeight="1">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -1998,7 +1985,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -2030,9 +2017,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="15.75" customHeight="1">
       <c r="A4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>46</v>
@@ -2059,9 +2046,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="15.75" customHeight="1">
       <c r="A5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>51</v>
@@ -2088,7 +2075,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="15.75" customHeight="1">
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -2111,16 +2098,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
@@ -2158,12 +2145,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1">
       <c r="A2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B2" t="s">
         <v>173</v>
-      </c>
-      <c r="B2" t="s">
-        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>